<commit_message>
Generar documentación Recibis en archivo zip
</commit_message>
<xml_diff>
--- a/documentacion/plantillas/gastos/Anexo XI-Bis Gastos Alumnos FP DUAL.xlsx
+++ b/documentacion/plantillas/gastos/Anexo XI-Bis Gastos Alumnos FP DUAL.xlsx
@@ -125,7 +125,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.00&quot; €&quot;"/>
     <numFmt numFmtId="168" formatCode="#,##0.00&quot; €&quot;;\-#,##0.00&quot; €&quot;"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -213,12 +213,6 @@
       <name val="Trebuchet MS"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -499,6 +493,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -534,10 +532,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -554,179 +548,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>105480</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>104760</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1054800</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5478840" y="6562440"/>
-          <a:ext cx="4086000" cy="980640"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="es-ES" sz="1000" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-            </a:rPr>
-            <a:t>EL/LA DIRECTOR/A</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="es-ES" sz="1000" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-            </a:rPr>
-            <a:t>	</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="es-ES" sz="1000" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-            </a:rPr>
-            <a:t>                EL TUTOR</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="es-ES" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr b="0" lang="es-ES" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr b="0" lang="es-ES" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr b="0" lang="es-ES" sz="1000" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Fdo:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="es-ES" sz="1000" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-            </a:rPr>
-            <a:t>	</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="es-ES" sz="1000" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-            </a:rPr>
-            <a:t>	</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="es-ES" sz="1000" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-              <a:ea typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Fdo:</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="es-ES" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:endParaRPr b="0" lang="es-ES" sz="1000" spc="-1" strike="noStrike">
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -734,8 +555,8 @@
   </sheetPr>
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -744,11 +565,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.85"/>
@@ -1338,51 +1160,50 @@
       <c r="E26" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="29"/>
-      <c r="I26" s="30" t="s">
+      <c r="G26" s="30"/>
+      <c r="H26" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="J26" s="31"/>
-      <c r="K26" s="32" t="s">
+      <c r="J26" s="32"/>
+      <c r="K26" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="L26" s="33" t="n">
+      <c r="L26" s="34" t="n">
         <f aca="false">SUM(L8:L25)</f>
         <v>0</v>
       </c>
-      <c r="M26" s="33"/>
+      <c r="M26" s="34"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="H27" s="29"/>
+      <c r="H27" s="30"/>
     </row>
     <row r="28" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="35" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D30" s="38"/>
-      <c r="E30" s="0" t="s">
+      <c r="D30" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="H30" s="39" t="s">
+      <c r="G30" s="39" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2419,7 +2240,6 @@
     <oddHeader>&amp;CCONSEJERÍA DE EDUCACIÓN,  CULTURA Y DEPORTES DIRECCIÓN GENERAL DE  PROGRAMAS, ATENCIÓN A LA DIVERSIDAD Y FORMACIÓN PROFESIONAL RESUMEN DE GASTOS EXTRAORDINARIOS DE ALUMNOS POR LA REALIZACIÓN DEL MÓDULO DE F.C.T.</oddHeader>
     <oddFooter>&amp;RPag. &amp;P de</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2431,7 +2251,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D26:I32 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3459,7 +3279,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D26:I32 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>